<commit_message>
weekly health report doc
</commit_message>
<xml_diff>
--- a/EEJ1_Document Checklist.xlsx
+++ b/EEJ1_Document Checklist.xlsx
@@ -64,9 +64,6 @@
     <t>EETeamJ1_ScrumTrackerSheet.xls</t>
   </si>
   <si>
-    <t>EEJ1_nagios_installation_and_montoring</t>
-  </si>
-  <si>
     <t>EEJ1_solution_architecture_document</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>c) Benchmarking testing</t>
+  </si>
+  <si>
+    <t>EEJ1_nagios_installation_and_montoring, EEJ1_Weekly_Health_Report</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +506,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,7 +514,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -530,7 +530,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -543,26 +543,26 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -573,7 +573,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -589,32 +589,32 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,7 +630,7 @@
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -649,10 +649,10 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>